<commit_message>
Add: place and break special
</commit_message>
<xml_diff>
--- a/assets/data/SheetTable.xlsx
+++ b/assets/data/SheetTable.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Avela\Pyxel\PyxelMeetsCraft\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C8944C-0BA2-4F17-908D-61A2D8F6F08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BB2726-43C1-4F5B-95A4-8643F676635A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
     <sheet name="Items" sheetId="2" r:id="rId2"/>
+    <sheet name="Craft" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -424,6 +425,141 @@
   </si>
   <si>
     <t>Shave</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Size_X</t>
+  </si>
+  <si>
+    <t>Size_Y</t>
+  </si>
+  <si>
+    <t>Shaped</t>
+  </si>
+  <si>
+    <t>Craft_0</t>
+  </si>
+  <si>
+    <t>Craft_1</t>
+  </si>
+  <si>
+    <t>Craft_2</t>
+  </si>
+  <si>
+    <t>Wood_Planks_block_item,Wood_Planks_block_item</t>
+  </si>
+  <si>
+    <t>Wood_Planks_block_item.Wood_Planks_block_item.Wood_Planks_block_item</t>
+  </si>
+  <si>
+    <t>Wood_Planks_block_item,null,Wood_Planks_block_item</t>
+  </si>
+  <si>
+    <t>Cobblestone_block_item,Cobblestone_block_item,Cobblestone_block_item</t>
+  </si>
+  <si>
+    <t>Cobblestone_block_item,null,Cobblestone_block_item</t>
+  </si>
+  <si>
+    <t>Wool_White_block_item,Wool_White_block_item,Wool_White_block_item</t>
+  </si>
+  <si>
+    <t>Wool_Black_block_item,Wool_Black_block_item,Wool_Black_block_item</t>
+  </si>
+  <si>
+    <t>Wool_Red_block_item,Wool_Red_block_item,Wool_Red_block_item</t>
+  </si>
+  <si>
+    <t>Wool_Yellow_block_item,Wool_Yellow_block_item,Wool_Yellow_block_item</t>
+  </si>
+  <si>
+    <t>Wool_Blue_block_item,Wool_Blue_block_item,Wool_Blue_block_item</t>
+  </si>
+  <si>
+    <t>Wool_Green_block_item,Wool_Green_block_item,Wool_Green_block_item</t>
+  </si>
+  <si>
+    <t>Diamond,Diamond,Diamond</t>
+  </si>
+  <si>
+    <t>Gold,Gold,Gold</t>
+  </si>
+  <si>
+    <t>Iron,Iron,Iron</t>
+  </si>
+  <si>
+    <t>Wood_Planks_block_item,Wood_Planks_block_item,Wood_Planks_block_item</t>
+  </si>
+  <si>
+    <t>null,Stick,null</t>
+  </si>
+  <si>
+    <t>Cobblestone_block_item,Cobblestone_block_item</t>
+  </si>
+  <si>
+    <t>Iron,Iron</t>
+  </si>
+  <si>
+    <t>Gold,Gold</t>
+  </si>
+  <si>
+    <t>Diamond,Diamond</t>
+  </si>
+  <si>
+    <t>null,Stick</t>
+  </si>
+  <si>
+    <t>Wood_Planks_block_item,Stick</t>
+  </si>
+  <si>
+    <t>Cobblestone_block_item,Stick</t>
+  </si>
+  <si>
+    <t>Iron,Stick</t>
+  </si>
+  <si>
+    <t>Gold,Stick</t>
+  </si>
+  <si>
+    <t>Diamond,Stick</t>
+  </si>
+  <si>
+    <t>Stick,Wood_Planks_block_item</t>
+  </si>
+  <si>
+    <t>Stick,Cobblestone_block_item</t>
+  </si>
+  <si>
+    <t>Stick,Iron</t>
+  </si>
+  <si>
+    <t>Stick,Diamond</t>
+  </si>
+  <si>
+    <t>Stick,Gold</t>
+  </si>
+  <si>
+    <t>Stick,null</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Shears</t>
+  </si>
+  <si>
+    <t>null,Iron</t>
+  </si>
+  <si>
+    <t>Iron,null</t>
+  </si>
+  <si>
+    <t>Special</t>
   </si>
 </sst>
 </file>
@@ -833,7 +969,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,7 +1633,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -1523,7 +1659,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -1549,7 +1685,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
@@ -1575,7 +1711,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -1761,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E204B5-2DBB-4D1D-8B6B-17C70CA7456E}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +2127,7 @@
         <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -2014,7 +2150,7 @@
         <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -2037,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -2060,7 +2196,7 @@
         <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -2671,10 +2807,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="C39" s="1">
         <v>5</v>
@@ -3457,7 +3593,7 @@
       <c r="B66" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="5">
         <v>0</v>
       </c>
       <c r="D66" s="1">
@@ -3542,7 +3678,7 @@
         <v>121</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C69" s="1">
         <v>0</v>
@@ -3571,7 +3707,7 @@
         <v>122</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C70" s="1">
         <v>0</v>
@@ -3599,4 +3735,1213 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC02698-AB06-4E47-BFA6-DBAF2D5E7097}">
+  <dimension ref="A1:H70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="50.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add: Move item in inventory
</commit_message>
<xml_diff>
--- a/assets/data/SheetTable.xlsx
+++ b/assets/data/SheetTable.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Avela\Pyxel\PyxelMeetsCraft\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A13D220-EE9E-4507-9EE7-95EBD56B6651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B4FD74-3A57-4AF0-A42F-DC11280B0C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Craft" sheetId="3" r:id="rId3"/>
+    <sheet name="Smelt" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -968,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE05F63-8377-4ACF-8A13-F43DF1F1C6BA}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -1897,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E204B5-2DBB-4D1D-8B6B-17C70CA7456E}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,7 +3743,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4944,4 +4945,214 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D32506-C071-4BF3-92EA-1CAD9496F7D0}">
+  <dimension ref="A1:B70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: craft infinity items
</commit_message>
<xml_diff>
--- a/assets/data/SheetTable.xlsx
+++ b/assets/data/SheetTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Avela\Pyxel\PyxelMeetsCraft\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC737E3E-8B81-42A4-8048-791B79260DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A34DD8-6F23-498D-8DF5-D9CD858E279A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -558,6 +558,9 @@
   </si>
   <si>
     <t>Special</t>
+  </si>
+  <si>
+    <t>Emerald,Emerald,Emerald</t>
   </si>
 </sst>
 </file>
@@ -966,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE05F63-8377-4ACF-8A13-F43DF1F1C6BA}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1895,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E204B5-2DBB-4D1D-8B6B-17C70CA7456E}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A55" activeCellId="3" sqref="A52 A53 A54 A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,8 +3742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC02698-AB06-4E47-BFA6-DBAF2D5E7097}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4824,7 +4827,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>169</v>
       </c>
@@ -4844,49 +4847,185 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="1">
+        <v>9</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="1">
+        <v>9</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="1">
+        <v>9</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="1">
+        <v>9</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix: furnance infinite items
</commit_message>
<xml_diff>
--- a/assets/data/SheetTable.xlsx
+++ b/assets/data/SheetTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Avela\Pyxel\PyxelMeetsCraft\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C57C2E-E9E8-440F-BD75-B34C3860701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26102C37-5C7C-49A2-BB6F-49BDD06C5C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D86D60BF-61DD-4416-8ABE-6AA53555BF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -564,6 +564,12 @@
   </si>
   <si>
     <t>Stone_block_item,Stone_block_item</t>
+  </si>
+  <si>
+    <t>Dirt_block_item,Leaves_block_item</t>
+  </si>
+  <si>
+    <t>Leaves_block_item,Dirt_block_item</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E204B5-2DBB-4D1D-8B6B-17C70CA7456E}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3850,8 +3856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC02698-AB06-4E47-BFA6-DBAF2D5E7097}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5136,19 +5142,88 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
+      <c r="A59" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>3</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
+      <c r="A60" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
+      <c r="A61" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
+      <c r="A62" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
+      <c r="G63" s="5"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>

</xml_diff>